<commit_message>
changes updated to git
</commit_message>
<xml_diff>
--- a/src/main/TestData/sagarTestFile.xlsx
+++ b/src/main/TestData/sagarTestFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>karan</t>
+  </si>
+  <si>
+    <t>Akbar</t>
+  </si>
+  <si>
+    <t>Tester#123</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,6 +465,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>